<commit_message>
Completed Test Cycle: Added Security Test Case (TC_010) and finalized logs
</commit_message>
<xml_diff>
--- a/test-cases/WISE (Web-based Institutional System for Education) - QA Test Execution Logs.xlsx
+++ b/test-cases/WISE (Web-based Institutional System for Education) - QA Test Execution Logs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="86">
   <si>
     <t>ID</t>
   </si>
@@ -251,6 +251,24 @@
   </si>
   <si>
     <t>4. Click "Create Course"</t>
+  </si>
+  <si>
+    <t>TC_010</t>
+  </si>
+  <si>
+    <t>Verify that User cannot access the Admin Dashboard via URL manipulation.</t>
+  </si>
+  <si>
+    <t>User is redirected to Home or Access Denied page</t>
+  </si>
+  <si>
+    <t>System successfully blocked access and redirected user back to Student Home.</t>
+  </si>
+  <si>
+    <t>2. Input Valid student account information for Logging in</t>
+  </si>
+  <si>
+    <t>3. Modify the current URL link by changing the route "/student/my-courses" to "/admin/analytics"</t>
   </si>
 </sst>
 </file>
@@ -567,8 +585,8 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="15.63"/>
     <col customWidth="1" min="2" max="2" width="27.5"/>
-    <col customWidth="1" min="3" max="3" width="51.13"/>
-    <col customWidth="1" min="4" max="4" width="61.5"/>
+    <col customWidth="1" min="3" max="3" width="68.0"/>
+    <col customWidth="1" min="4" max="4" width="79.13"/>
     <col customWidth="1" min="5" max="5" width="57.13"/>
     <col customWidth="1" min="6" max="6" width="73.13"/>
     <col customWidth="1" min="7" max="7" width="12.88"/>
@@ -2327,13 +2345,27 @@
       <c r="Z55" s="3"/>
     </row>
     <row r="56">
-      <c r="A56" s="4"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
+      <c r="A56" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
@@ -2358,7 +2390,9 @@
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
-      <c r="D57" s="8"/>
+      <c r="D57" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
@@ -2386,7 +2420,9 @@
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
-      <c r="D58" s="8"/>
+      <c r="D58" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>

</xml_diff>